<commit_message>
changes in the datatool and excel files
</commit_message>
<xml_diff>
--- a/files/DxH_ConfigImport_Veniano_HA.xlsx
+++ b/files/DxH_ConfigImport_Veniano_HA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rf128sp\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5667204D-DBAC-4323-97AA-EDB1BC76BD84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80E463F-1A5A-444A-BA52-05043E153480}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dtreason" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="commonparameterstest" sheetId="5" r:id="rId5"/>
     <sheet name="uom" sheetId="6" r:id="rId6"/>
     <sheet name="unavailable" sheetId="7" r:id="rId7"/>
+    <sheet name="tfdusers" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="230">
   <si>
     <t>asset_code</t>
   </si>
@@ -469,6 +470,258 @@
   </si>
   <si>
     <t xml:space="preserve">Meter </t>
+  </si>
+  <si>
+    <t>Badge</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Abu</t>
+  </si>
+  <si>
+    <t>Tabl Mohamed Aly Abd El F</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Andriotta</t>
+  </si>
+  <si>
+    <t>Giorgio</t>
+  </si>
+  <si>
+    <t>Annoni</t>
+  </si>
+  <si>
+    <t>Salvatore</t>
+  </si>
+  <si>
+    <t>Badalamenti</t>
+  </si>
+  <si>
+    <t>Samuele</t>
+  </si>
+  <si>
+    <t>Bazzoni</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Brancati</t>
+  </si>
+  <si>
+    <t>Emanuele</t>
+  </si>
+  <si>
+    <t>Branco</t>
+  </si>
+  <si>
+    <t>Gerardo Doriano</t>
+  </si>
+  <si>
+    <t>Capezzera</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Casino</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Cassinelli</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Castelvedere</t>
+  </si>
+  <si>
+    <t>Barbara</t>
+  </si>
+  <si>
+    <t>Ceccarello</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>Domenico</t>
+  </si>
+  <si>
+    <t>Torre Simone</t>
+  </si>
+  <si>
+    <t>Della</t>
+  </si>
+  <si>
+    <t>Daniele Francesco</t>
+  </si>
+  <si>
+    <t>Di Falco</t>
+  </si>
+  <si>
+    <t>Luigi</t>
+  </si>
+  <si>
+    <t>Doninelli</t>
+  </si>
+  <si>
+    <t>Adriano</t>
+  </si>
+  <si>
+    <t>Filia</t>
+  </si>
+  <si>
+    <t>Simone</t>
+  </si>
+  <si>
+    <t>Gilg</t>
+  </si>
+  <si>
+    <t>Gornati</t>
+  </si>
+  <si>
+    <t>Matteo</t>
+  </si>
+  <si>
+    <t>Grieco</t>
+  </si>
+  <si>
+    <t>Michele</t>
+  </si>
+  <si>
+    <t>Intorto</t>
+  </si>
+  <si>
+    <t>Massimiliano</t>
+  </si>
+  <si>
+    <t>Lombardi</t>
+  </si>
+  <si>
+    <t>Antonino</t>
+  </si>
+  <si>
+    <t>Maceli</t>
+  </si>
+  <si>
+    <t>Giuseppe</t>
+  </si>
+  <si>
+    <t>Marino</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Melara</t>
+  </si>
+  <si>
+    <t>Candelario Hamilton Steven</t>
+  </si>
+  <si>
+    <t>Munoz</t>
+  </si>
+  <si>
+    <t>Negretti</t>
+  </si>
+  <si>
+    <t>Nicosia</t>
+  </si>
+  <si>
+    <t>Parrotta</t>
+  </si>
+  <si>
+    <t>Faustino</t>
+  </si>
+  <si>
+    <t>Pini</t>
+  </si>
+  <si>
+    <t>Quarticelli</t>
+  </si>
+  <si>
+    <t>Gerardo</t>
+  </si>
+  <si>
+    <t>Rizzi</t>
+  </si>
+  <si>
+    <t>Gabriele</t>
+  </si>
+  <si>
+    <t>Ronchi</t>
+  </si>
+  <si>
+    <t>Amadou Mactar</t>
+  </si>
+  <si>
+    <t>Sall</t>
+  </si>
+  <si>
+    <t>Alfonso</t>
+  </si>
+  <si>
+    <t>Sansone</t>
+  </si>
+  <si>
+    <t>Paolo</t>
+  </si>
+  <si>
+    <t>Spinello</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Tubelli</t>
+  </si>
+  <si>
+    <t>Pagani</t>
+  </si>
+  <si>
+    <t>Giovani</t>
+  </si>
+  <si>
+    <t>Roberto</t>
+  </si>
+  <si>
+    <t>Fedeli</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>DAlessandro</t>
+  </si>
+  <si>
+    <t>Darrigo</t>
   </si>
 </sst>
 </file>
@@ -533,7 +786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -546,6 +799,18 @@
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8668,7 +8933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
@@ -13062,4 +13327,910 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868E2915-FB4F-49BC-B896-6E22979130DF}">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2260</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2279</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2283</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2259</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2275</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2255</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2239</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2250</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2252</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2240</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2247</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2291</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2246</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2238</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2265</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2242</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="8">
+        <v>2261</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2267</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2248</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="8">
+        <v>2256</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2286</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="8">
+        <v>2251</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="8">
+        <v>2245</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" s="8">
+        <v>2254</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8">
+        <v>2264</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="8">
+        <v>2280</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="8">
+        <v>2285</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="8">
+        <v>2284</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" s="8">
+        <v>2277</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G30" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" s="8">
+        <v>2253</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G31" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" s="8">
+        <v>2262</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G32" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="8">
+        <v>2243</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G33" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" s="8">
+        <v>2249</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2258</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="8">
+        <v>2266</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G36" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="8">
+        <v>2241</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="8">
+        <v>2268</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" s="8">
+        <v>2276</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G39" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" s="8">
+        <v>2257</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" s="8">
+        <v>1169</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G41" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" s="13">
+        <v>1886</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G42" s="11">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes in the import feature
</commit_message>
<xml_diff>
--- a/files/DxH_ConfigImport_Veniano_HA.xlsx
+++ b/files/DxH_ConfigImport_Veniano_HA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rf128sp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rf128sp\ADV-DXH\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80E463F-1A5A-444A-BA52-05043E153480}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6591B280-5EA1-4655-A697-CC05FF6B40B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="asset" sheetId="2" r:id="rId2"/>
     <sheet name="shift" sheetId="3" r:id="rId3"/>
     <sheet name="tag" sheetId="4" r:id="rId4"/>
-    <sheet name="commonparameterstest" sheetId="5" r:id="rId5"/>
+    <sheet name="commonparameters" sheetId="5" r:id="rId5"/>
     <sheet name="uom" sheetId="6" r:id="rId6"/>
     <sheet name="unavailable" sheetId="7" r:id="rId7"/>
     <sheet name="tfdusers" sheetId="8" r:id="rId8"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="244">
   <si>
     <t>asset_code</t>
   </si>
@@ -722,6 +722,48 @@
   </si>
   <si>
     <t>Darrigo</t>
+  </si>
+  <si>
+    <t>168H-0001.Cutter.Count</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>2019-12-17 00:00:00.000</t>
+  </si>
+  <si>
+    <t>168H-0004.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0005.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0006.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0007.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0008.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0009.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0010.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0011.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0013.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0002.Cutter.Count</t>
+  </si>
+  <si>
+    <t>168H-0003.Cutter.Count</t>
   </si>
 </sst>
 </file>
@@ -1127,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="M210" sqref="M210:M222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1262,7 @@
         <v>106</v>
       </c>
       <c r="M2">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1255,7 +1297,7 @@
         <v>106</v>
       </c>
       <c r="M3">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1290,7 +1332,7 @@
         <v>106</v>
       </c>
       <c r="M4">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1325,7 +1367,7 @@
         <v>106</v>
       </c>
       <c r="M5">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1360,7 +1402,7 @@
         <v>106</v>
       </c>
       <c r="M6">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1395,7 +1437,7 @@
         <v>106</v>
       </c>
       <c r="M7">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1430,7 +1472,7 @@
         <v>106</v>
       </c>
       <c r="M8">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1465,7 +1507,7 @@
         <v>106</v>
       </c>
       <c r="M9">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1500,7 +1542,7 @@
         <v>106</v>
       </c>
       <c r="M10">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1535,7 +1577,7 @@
         <v>106</v>
       </c>
       <c r="M11">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1570,7 +1612,7 @@
         <v>106</v>
       </c>
       <c r="M12">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1605,7 +1647,7 @@
         <v>106</v>
       </c>
       <c r="M13">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1640,7 +1682,7 @@
         <v>106</v>
       </c>
       <c r="M14">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1675,7 +1717,7 @@
         <v>106</v>
       </c>
       <c r="M15">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1710,7 +1752,7 @@
         <v>106</v>
       </c>
       <c r="M16">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1745,7 +1787,7 @@
         <v>106</v>
       </c>
       <c r="M17">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1780,7 +1822,7 @@
         <v>106</v>
       </c>
       <c r="M18">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1815,7 +1857,7 @@
         <v>106</v>
       </c>
       <c r="M19">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1850,7 +1892,7 @@
         <v>106</v>
       </c>
       <c r="M20">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1885,7 +1927,7 @@
         <v>106</v>
       </c>
       <c r="M21">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1920,7 +1962,7 @@
         <v>106</v>
       </c>
       <c r="M22">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1955,7 +1997,7 @@
         <v>106</v>
       </c>
       <c r="M23">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1990,7 +2032,7 @@
         <v>106</v>
       </c>
       <c r="M24">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2025,7 +2067,7 @@
         <v>106</v>
       </c>
       <c r="M25">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2060,7 +2102,7 @@
         <v>106</v>
       </c>
       <c r="M26">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2095,7 +2137,7 @@
         <v>106</v>
       </c>
       <c r="M27">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2130,7 +2172,7 @@
         <v>106</v>
       </c>
       <c r="M28">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2165,7 +2207,7 @@
         <v>106</v>
       </c>
       <c r="M29">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2200,7 +2242,7 @@
         <v>106</v>
       </c>
       <c r="M30">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2235,7 +2277,7 @@
         <v>106</v>
       </c>
       <c r="M31">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2270,7 +2312,7 @@
         <v>106</v>
       </c>
       <c r="M32">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -2305,7 +2347,7 @@
         <v>106</v>
       </c>
       <c r="M33">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2340,7 +2382,7 @@
         <v>106</v>
       </c>
       <c r="M34">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2375,7 +2417,7 @@
         <v>106</v>
       </c>
       <c r="M35">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2410,7 +2452,7 @@
         <v>106</v>
       </c>
       <c r="M36">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2445,7 +2487,7 @@
         <v>106</v>
       </c>
       <c r="M37">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2480,7 +2522,7 @@
         <v>106</v>
       </c>
       <c r="M38">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2515,7 +2557,7 @@
         <v>106</v>
       </c>
       <c r="M39">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2550,7 +2592,7 @@
         <v>106</v>
       </c>
       <c r="M40">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2585,7 +2627,7 @@
         <v>106</v>
       </c>
       <c r="M41">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2620,7 +2662,7 @@
         <v>106</v>
       </c>
       <c r="M42">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2655,7 +2697,7 @@
         <v>106</v>
       </c>
       <c r="M43">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2690,7 +2732,7 @@
         <v>106</v>
       </c>
       <c r="M44">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2725,7 +2767,7 @@
         <v>106</v>
       </c>
       <c r="M45">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -2760,7 +2802,7 @@
         <v>106</v>
       </c>
       <c r="M46">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2795,7 +2837,7 @@
         <v>106</v>
       </c>
       <c r="M47">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2830,7 +2872,7 @@
         <v>106</v>
       </c>
       <c r="M48">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -2865,7 +2907,7 @@
         <v>106</v>
       </c>
       <c r="M49">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2900,7 +2942,7 @@
         <v>106</v>
       </c>
       <c r="M50">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2935,7 +2977,7 @@
         <v>106</v>
       </c>
       <c r="M51">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -2970,7 +3012,7 @@
         <v>106</v>
       </c>
       <c r="M52">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3005,7 +3047,7 @@
         <v>106</v>
       </c>
       <c r="M53">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3040,7 +3082,7 @@
         <v>106</v>
       </c>
       <c r="M54">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3075,7 +3117,7 @@
         <v>106</v>
       </c>
       <c r="M55">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3110,7 +3152,7 @@
         <v>106</v>
       </c>
       <c r="M56">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3145,7 +3187,7 @@
         <v>106</v>
       </c>
       <c r="M57">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3180,7 +3222,7 @@
         <v>106</v>
       </c>
       <c r="M58">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -3215,7 +3257,7 @@
         <v>106</v>
       </c>
       <c r="M59">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -3250,7 +3292,7 @@
         <v>106</v>
       </c>
       <c r="M60">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3285,7 +3327,7 @@
         <v>106</v>
       </c>
       <c r="M61">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3320,7 +3362,7 @@
         <v>106</v>
       </c>
       <c r="M62">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3355,7 +3397,7 @@
         <v>106</v>
       </c>
       <c r="M63">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3390,7 +3432,7 @@
         <v>106</v>
       </c>
       <c r="M64">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -3425,7 +3467,7 @@
         <v>106</v>
       </c>
       <c r="M65">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -3460,7 +3502,7 @@
         <v>106</v>
       </c>
       <c r="M66">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3495,7 +3537,7 @@
         <v>106</v>
       </c>
       <c r="M67">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -3530,7 +3572,7 @@
         <v>106</v>
       </c>
       <c r="M68">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -3565,7 +3607,7 @@
         <v>106</v>
       </c>
       <c r="M69">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -3600,7 +3642,7 @@
         <v>106</v>
       </c>
       <c r="M70">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -3635,7 +3677,7 @@
         <v>106</v>
       </c>
       <c r="M71">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -3670,7 +3712,7 @@
         <v>106</v>
       </c>
       <c r="M72">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -3705,7 +3747,7 @@
         <v>106</v>
       </c>
       <c r="M73">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -3740,7 +3782,7 @@
         <v>106</v>
       </c>
       <c r="M74">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -3775,7 +3817,7 @@
         <v>106</v>
       </c>
       <c r="M75">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -3810,7 +3852,7 @@
         <v>106</v>
       </c>
       <c r="M76">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -3845,7 +3887,7 @@
         <v>106</v>
       </c>
       <c r="M77">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -3880,7 +3922,7 @@
         <v>106</v>
       </c>
       <c r="M78">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -3915,7 +3957,7 @@
         <v>106</v>
       </c>
       <c r="M79">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -3950,7 +3992,7 @@
         <v>106</v>
       </c>
       <c r="M80">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -3985,7 +4027,7 @@
         <v>106</v>
       </c>
       <c r="M81">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4020,7 +4062,7 @@
         <v>106</v>
       </c>
       <c r="M82">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4055,7 +4097,7 @@
         <v>106</v>
       </c>
       <c r="M83">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4090,7 +4132,7 @@
         <v>106</v>
       </c>
       <c r="M84">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -4125,7 +4167,7 @@
         <v>106</v>
       </c>
       <c r="M85">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -4160,7 +4202,7 @@
         <v>106</v>
       </c>
       <c r="M86">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -4195,7 +4237,7 @@
         <v>106</v>
       </c>
       <c r="M87">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -4230,7 +4272,7 @@
         <v>106</v>
       </c>
       <c r="M88">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -4265,7 +4307,7 @@
         <v>106</v>
       </c>
       <c r="M89">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -4300,7 +4342,7 @@
         <v>106</v>
       </c>
       <c r="M90">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -4335,7 +4377,7 @@
         <v>106</v>
       </c>
       <c r="M91">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -4370,7 +4412,7 @@
         <v>106</v>
       </c>
       <c r="M92">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -4405,7 +4447,7 @@
         <v>106</v>
       </c>
       <c r="M93">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -4440,7 +4482,7 @@
         <v>106</v>
       </c>
       <c r="M94">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -4475,7 +4517,7 @@
         <v>106</v>
       </c>
       <c r="M95">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -4510,7 +4552,7 @@
         <v>106</v>
       </c>
       <c r="M96">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -4545,7 +4587,7 @@
         <v>106</v>
       </c>
       <c r="M97">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4580,7 +4622,7 @@
         <v>106</v>
       </c>
       <c r="M98">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4615,7 +4657,7 @@
         <v>106</v>
       </c>
       <c r="M99">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4650,7 +4692,7 @@
         <v>106</v>
       </c>
       <c r="M100">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -4685,7 +4727,7 @@
         <v>106</v>
       </c>
       <c r="M101">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -4720,7 +4762,7 @@
         <v>106</v>
       </c>
       <c r="M102">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -4755,7 +4797,7 @@
         <v>106</v>
       </c>
       <c r="M103">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -4790,7 +4832,7 @@
         <v>106</v>
       </c>
       <c r="M104">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -4825,7 +4867,7 @@
         <v>106</v>
       </c>
       <c r="M105">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -4860,7 +4902,7 @@
         <v>106</v>
       </c>
       <c r="M106">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -4895,7 +4937,7 @@
         <v>106</v>
       </c>
       <c r="M107">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -4930,7 +4972,7 @@
         <v>106</v>
       </c>
       <c r="M108">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -4965,7 +5007,7 @@
         <v>106</v>
       </c>
       <c r="M109">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -5000,7 +5042,7 @@
         <v>106</v>
       </c>
       <c r="M110">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -5035,7 +5077,7 @@
         <v>106</v>
       </c>
       <c r="M111">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -5070,7 +5112,7 @@
         <v>106</v>
       </c>
       <c r="M112">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -5105,7 +5147,7 @@
         <v>106</v>
       </c>
       <c r="M113">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -5140,7 +5182,7 @@
         <v>106</v>
       </c>
       <c r="M114">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -5175,7 +5217,7 @@
         <v>106</v>
       </c>
       <c r="M115">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -5210,7 +5252,7 @@
         <v>106</v>
       </c>
       <c r="M116">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -5245,7 +5287,7 @@
         <v>106</v>
       </c>
       <c r="M117">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -5280,7 +5322,7 @@
         <v>106</v>
       </c>
       <c r="M118">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -5315,7 +5357,7 @@
         <v>106</v>
       </c>
       <c r="M119">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -5350,7 +5392,7 @@
         <v>106</v>
       </c>
       <c r="M120">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -5385,7 +5427,7 @@
         <v>106</v>
       </c>
       <c r="M121">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -5420,7 +5462,7 @@
         <v>106</v>
       </c>
       <c r="M122">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -5455,7 +5497,7 @@
         <v>106</v>
       </c>
       <c r="M123">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -5490,7 +5532,7 @@
         <v>106</v>
       </c>
       <c r="M124">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -5525,7 +5567,7 @@
         <v>106</v>
       </c>
       <c r="M125">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -5560,7 +5602,7 @@
         <v>106</v>
       </c>
       <c r="M126">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
@@ -5595,7 +5637,7 @@
         <v>106</v>
       </c>
       <c r="M127">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
@@ -5630,7 +5672,7 @@
         <v>106</v>
       </c>
       <c r="M128">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -5665,7 +5707,7 @@
         <v>106</v>
       </c>
       <c r="M129">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -5700,7 +5742,7 @@
         <v>106</v>
       </c>
       <c r="M130">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -5735,7 +5777,7 @@
         <v>106</v>
       </c>
       <c r="M131">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -5770,7 +5812,7 @@
         <v>106</v>
       </c>
       <c r="M132">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -5805,7 +5847,7 @@
         <v>106</v>
       </c>
       <c r="M133">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -5840,7 +5882,7 @@
         <v>106</v>
       </c>
       <c r="M134">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -5875,7 +5917,7 @@
         <v>106</v>
       </c>
       <c r="M135">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -5910,7 +5952,7 @@
         <v>106</v>
       </c>
       <c r="M136">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -5945,7 +5987,7 @@
         <v>106</v>
       </c>
       <c r="M137">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
@@ -5980,7 +6022,7 @@
         <v>106</v>
       </c>
       <c r="M138">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -6015,7 +6057,7 @@
         <v>106</v>
       </c>
       <c r="M139">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
@@ -6050,7 +6092,7 @@
         <v>106</v>
       </c>
       <c r="M140">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -6085,7 +6127,7 @@
         <v>106</v>
       </c>
       <c r="M141">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
@@ -6120,7 +6162,7 @@
         <v>106</v>
       </c>
       <c r="M142">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
@@ -6155,7 +6197,7 @@
         <v>106</v>
       </c>
       <c r="M143">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -6190,7 +6232,7 @@
         <v>106</v>
       </c>
       <c r="M144">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
@@ -6225,7 +6267,7 @@
         <v>106</v>
       </c>
       <c r="M145">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -6260,7 +6302,7 @@
         <v>106</v>
       </c>
       <c r="M146">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
@@ -6295,7 +6337,7 @@
         <v>106</v>
       </c>
       <c r="M147">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -6330,7 +6372,7 @@
         <v>106</v>
       </c>
       <c r="M148">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -6365,7 +6407,7 @@
         <v>106</v>
       </c>
       <c r="M149">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -6400,7 +6442,7 @@
         <v>106</v>
       </c>
       <c r="M150">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -6435,7 +6477,7 @@
         <v>106</v>
       </c>
       <c r="M151">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
@@ -6470,7 +6512,7 @@
         <v>106</v>
       </c>
       <c r="M152">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -6505,7 +6547,7 @@
         <v>106</v>
       </c>
       <c r="M153">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -6540,7 +6582,7 @@
         <v>106</v>
       </c>
       <c r="M154">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -6575,7 +6617,7 @@
         <v>106</v>
       </c>
       <c r="M155">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
@@ -6610,7 +6652,7 @@
         <v>106</v>
       </c>
       <c r="M156">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
@@ -6645,7 +6687,7 @@
         <v>106</v>
       </c>
       <c r="M157">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
@@ -6680,7 +6722,7 @@
         <v>106</v>
       </c>
       <c r="M158">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
@@ -6715,7 +6757,7 @@
         <v>106</v>
       </c>
       <c r="M159">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
@@ -6750,7 +6792,7 @@
         <v>106</v>
       </c>
       <c r="M160">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
@@ -6785,7 +6827,7 @@
         <v>106</v>
       </c>
       <c r="M161">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
@@ -6820,7 +6862,7 @@
         <v>106</v>
       </c>
       <c r="M162">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
@@ -6855,7 +6897,7 @@
         <v>106</v>
       </c>
       <c r="M163">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
@@ -6890,7 +6932,7 @@
         <v>106</v>
       </c>
       <c r="M164">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
@@ -6925,7 +6967,7 @@
         <v>106</v>
       </c>
       <c r="M165">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
@@ -6960,7 +7002,7 @@
         <v>106</v>
       </c>
       <c r="M166">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -6995,7 +7037,7 @@
         <v>106</v>
       </c>
       <c r="M167">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -7030,7 +7072,7 @@
         <v>106</v>
       </c>
       <c r="M168">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -7065,7 +7107,7 @@
         <v>106</v>
       </c>
       <c r="M169">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -7100,7 +7142,7 @@
         <v>106</v>
       </c>
       <c r="M170">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -7135,7 +7177,7 @@
         <v>106</v>
       </c>
       <c r="M171">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
@@ -7170,7 +7212,7 @@
         <v>106</v>
       </c>
       <c r="M172">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -7205,7 +7247,7 @@
         <v>106</v>
       </c>
       <c r="M173">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -7240,7 +7282,7 @@
         <v>106</v>
       </c>
       <c r="M174">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
@@ -7275,7 +7317,7 @@
         <v>106</v>
       </c>
       <c r="M175">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
@@ -7310,7 +7352,7 @@
         <v>106</v>
       </c>
       <c r="M176">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
@@ -7345,7 +7387,7 @@
         <v>106</v>
       </c>
       <c r="M177">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
@@ -7380,7 +7422,7 @@
         <v>106</v>
       </c>
       <c r="M178">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
@@ -7415,7 +7457,7 @@
         <v>106</v>
       </c>
       <c r="M179">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
@@ -7450,7 +7492,7 @@
         <v>106</v>
       </c>
       <c r="M180">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
@@ -7485,7 +7527,7 @@
         <v>106</v>
       </c>
       <c r="M181">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
@@ -7520,7 +7562,7 @@
         <v>106</v>
       </c>
       <c r="M182">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
@@ -7555,7 +7597,7 @@
         <v>106</v>
       </c>
       <c r="M183">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
@@ -7590,7 +7632,7 @@
         <v>106</v>
       </c>
       <c r="M184">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
@@ -7625,7 +7667,7 @@
         <v>106</v>
       </c>
       <c r="M185">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
@@ -7660,7 +7702,7 @@
         <v>106</v>
       </c>
       <c r="M186">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
@@ -7695,7 +7737,7 @@
         <v>106</v>
       </c>
       <c r="M187">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
@@ -7730,7 +7772,7 @@
         <v>106</v>
       </c>
       <c r="M188">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
@@ -7765,7 +7807,7 @@
         <v>106</v>
       </c>
       <c r="M189">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
@@ -7800,7 +7842,7 @@
         <v>106</v>
       </c>
       <c r="M190">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
@@ -7835,7 +7877,7 @@
         <v>106</v>
       </c>
       <c r="M191">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
@@ -7870,7 +7912,7 @@
         <v>106</v>
       </c>
       <c r="M192">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
@@ -7905,7 +7947,7 @@
         <v>106</v>
       </c>
       <c r="M193">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
@@ -7940,7 +7982,7 @@
         <v>106</v>
       </c>
       <c r="M194">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
@@ -7975,7 +8017,7 @@
         <v>106</v>
       </c>
       <c r="M195">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
@@ -8010,7 +8052,7 @@
         <v>106</v>
       </c>
       <c r="M196">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
@@ -8045,7 +8087,7 @@
         <v>106</v>
       </c>
       <c r="M197">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
@@ -8080,7 +8122,7 @@
         <v>106</v>
       </c>
       <c r="M198">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
@@ -8115,7 +8157,7 @@
         <v>106</v>
       </c>
       <c r="M199">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
@@ -8150,7 +8192,7 @@
         <v>106</v>
       </c>
       <c r="M200">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
@@ -8185,7 +8227,7 @@
         <v>106</v>
       </c>
       <c r="M201">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
@@ -8220,7 +8262,7 @@
         <v>106</v>
       </c>
       <c r="M202">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
@@ -8255,7 +8297,7 @@
         <v>106</v>
       </c>
       <c r="M203">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
@@ -8290,7 +8332,7 @@
         <v>106</v>
       </c>
       <c r="M204">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
@@ -8325,7 +8367,7 @@
         <v>106</v>
       </c>
       <c r="M205">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
@@ -8360,7 +8402,7 @@
         <v>106</v>
       </c>
       <c r="M206">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
@@ -8395,7 +8437,7 @@
         <v>106</v>
       </c>
       <c r="M207">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
@@ -8430,7 +8472,7 @@
         <v>106</v>
       </c>
       <c r="M208">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
@@ -8465,7 +8507,7 @@
         <v>106</v>
       </c>
       <c r="M209">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
@@ -8500,7 +8542,7 @@
         <v>106</v>
       </c>
       <c r="M210">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
@@ -8535,7 +8577,7 @@
         <v>106</v>
       </c>
       <c r="M211">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
@@ -8570,7 +8612,7 @@
         <v>106</v>
       </c>
       <c r="M212">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
@@ -8605,7 +8647,7 @@
         <v>106</v>
       </c>
       <c r="M213">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
@@ -8640,7 +8682,7 @@
         <v>106</v>
       </c>
       <c r="M214">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
@@ -8675,7 +8717,7 @@
         <v>106</v>
       </c>
       <c r="M215">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
@@ -8710,7 +8752,7 @@
         <v>106</v>
       </c>
       <c r="M216">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
@@ -8745,7 +8787,7 @@
         <v>106</v>
       </c>
       <c r="M217">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
@@ -8780,7 +8822,7 @@
         <v>106</v>
       </c>
       <c r="M218">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.25">
@@ -8815,7 +8857,7 @@
         <v>106</v>
       </c>
       <c r="M219">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.25">
@@ -8850,7 +8892,7 @@
         <v>106</v>
       </c>
       <c r="M220">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.25">
@@ -8885,7 +8927,7 @@
         <v>106</v>
       </c>
       <c r="M221">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.25">
@@ -8920,7 +8962,7 @@
         <v>106</v>
       </c>
       <c r="M222">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -9803,7 +9845,7 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9930,7 +9972,7 @@
         <v>106</v>
       </c>
       <c r="R2">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -9980,7 +10022,7 @@
         <v>106</v>
       </c>
       <c r="R3">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -9994,15 +10036,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="89.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -10017,7 +10060,7 @@
     <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
@@ -10064,25 +10107,34 @@
         <v>39</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>230</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>231</v>
+      </c>
+      <c r="E2" t="s">
+        <v>231</v>
       </c>
       <c r="F2" t="s">
         <v>61</v>
       </c>
+      <c r="G2" t="s">
+        <v>231</v>
+      </c>
       <c r="H2" t="s">
         <v>64</v>
       </c>
@@ -10099,16 +10151,655 @@
         <v>63</v>
       </c>
       <c r="M2" t="s">
-        <v>106</v>
+        <v>232</v>
       </c>
       <c r="N2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="O2" t="s">
-        <v>106</v>
+        <v>232</v>
       </c>
       <c r="P2">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="Q2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3">
+        <v>999999</v>
+      </c>
+      <c r="J3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" t="s">
+        <v>232</v>
+      </c>
+      <c r="N3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" t="s">
+        <v>232</v>
+      </c>
+      <c r="P3">
+        <v>119</v>
+      </c>
+      <c r="Q3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>231</v>
+      </c>
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4">
+        <v>999999</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" t="s">
+        <v>232</v>
+      </c>
+      <c r="N4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" t="s">
+        <v>232</v>
+      </c>
+      <c r="P4">
+        <v>119</v>
+      </c>
+      <c r="Q4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5">
+        <v>999999</v>
+      </c>
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" t="s">
+        <v>232</v>
+      </c>
+      <c r="N5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" t="s">
+        <v>232</v>
+      </c>
+      <c r="P5">
+        <v>119</v>
+      </c>
+      <c r="Q5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>231</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6">
+        <v>999999</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" t="s">
+        <v>232</v>
+      </c>
+      <c r="N6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" t="s">
+        <v>232</v>
+      </c>
+      <c r="P6">
+        <v>119</v>
+      </c>
+      <c r="Q6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7">
+        <v>999999</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" t="s">
+        <v>232</v>
+      </c>
+      <c r="N7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" t="s">
+        <v>232</v>
+      </c>
+      <c r="P7">
+        <v>119</v>
+      </c>
+      <c r="Q7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D8" t="s">
+        <v>231</v>
+      </c>
+      <c r="E8" t="s">
+        <v>231</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>231</v>
+      </c>
+      <c r="H8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8">
+        <v>999999</v>
+      </c>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" t="s">
+        <v>232</v>
+      </c>
+      <c r="N8" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" t="s">
+        <v>232</v>
+      </c>
+      <c r="P8">
+        <v>119</v>
+      </c>
+      <c r="Q8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" t="s">
+        <v>231</v>
+      </c>
+      <c r="E9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>231</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9">
+        <v>999999</v>
+      </c>
+      <c r="J9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" t="s">
+        <v>232</v>
+      </c>
+      <c r="N9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O9" t="s">
+        <v>232</v>
+      </c>
+      <c r="P9">
+        <v>119</v>
+      </c>
+      <c r="Q9">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" t="s">
+        <v>231</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10">
+        <v>999999</v>
+      </c>
+      <c r="J10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" t="s">
+        <v>232</v>
+      </c>
+      <c r="N10" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" t="s">
+        <v>232</v>
+      </c>
+      <c r="P10">
+        <v>119</v>
+      </c>
+      <c r="Q10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>231</v>
+      </c>
+      <c r="H11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11">
+        <v>999999</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" t="s">
+        <v>232</v>
+      </c>
+      <c r="N11" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11" t="s">
+        <v>232</v>
+      </c>
+      <c r="P11">
+        <v>119</v>
+      </c>
+      <c r="Q11">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E12" t="s">
+        <v>231</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12">
+        <v>999999</v>
+      </c>
+      <c r="J12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" t="s">
+        <v>232</v>
+      </c>
+      <c r="N12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O12" t="s">
+        <v>232</v>
+      </c>
+      <c r="P12">
+        <v>119</v>
+      </c>
+      <c r="Q12">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13" t="s">
+        <v>231</v>
+      </c>
+      <c r="E13" t="s">
+        <v>231</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>231</v>
+      </c>
+      <c r="H13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13">
+        <v>999999</v>
+      </c>
+      <c r="J13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" t="s">
+        <v>232</v>
+      </c>
+      <c r="N13" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" t="s">
+        <v>232</v>
+      </c>
+      <c r="P13">
+        <v>119</v>
+      </c>
+      <c r="Q13">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="s">
+        <v>231</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>231</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14">
+        <v>999999</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" t="s">
+        <v>106</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" t="s">
+        <v>232</v>
+      </c>
+      <c r="P14">
+        <v>119</v>
+      </c>
+      <c r="Q14">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -10121,19 +10812,22 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -10204,7 +10898,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>66</v>
@@ -10267,8 +10961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10344,7 +11038,7 @@
         <v>106</v>
       </c>
       <c r="J2">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -10357,7 +11051,7 @@
   <dimension ref="A1:O726"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13333,8 +14027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868E2915-FB4F-49BC-B896-6E22979130DF}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13387,7 +14081,7 @@
         <v>150</v>
       </c>
       <c r="G2" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -13408,7 +14102,7 @@
         <v>150</v>
       </c>
       <c r="G3" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -13429,7 +14123,7 @@
         <v>150</v>
       </c>
       <c r="G4" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -13450,7 +14144,7 @@
         <v>150</v>
       </c>
       <c r="G5" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -13471,7 +14165,7 @@
         <v>150</v>
       </c>
       <c r="G6" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -13492,7 +14186,7 @@
         <v>150</v>
       </c>
       <c r="G7" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -13513,7 +14207,7 @@
         <v>150</v>
       </c>
       <c r="G8" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -13534,7 +14228,7 @@
         <v>150</v>
       </c>
       <c r="G9" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -13555,7 +14249,7 @@
         <v>167</v>
       </c>
       <c r="G10" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -13576,7 +14270,7 @@
         <v>150</v>
       </c>
       <c r="G11" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -13597,7 +14291,7 @@
         <v>150</v>
       </c>
       <c r="G12" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -13618,7 +14312,7 @@
         <v>150</v>
       </c>
       <c r="G13" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -13639,7 +14333,7 @@
         <v>150</v>
       </c>
       <c r="G14" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -13660,7 +14354,7 @@
         <v>150</v>
       </c>
       <c r="G15" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -13681,7 +14375,7 @@
         <v>150</v>
       </c>
       <c r="G16" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -13702,7 +14396,7 @@
         <v>167</v>
       </c>
       <c r="G17" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -13723,7 +14417,7 @@
         <v>150</v>
       </c>
       <c r="G18" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -13744,7 +14438,7 @@
         <v>150</v>
       </c>
       <c r="G19" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -13765,7 +14459,7 @@
         <v>150</v>
       </c>
       <c r="G20" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -13786,7 +14480,7 @@
         <v>150</v>
       </c>
       <c r="G21" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -13807,7 +14501,7 @@
         <v>150</v>
       </c>
       <c r="G22" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -13828,7 +14522,7 @@
         <v>150</v>
       </c>
       <c r="G23" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -13849,7 +14543,7 @@
         <v>150</v>
       </c>
       <c r="G24" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -13870,7 +14564,7 @@
         <v>150</v>
       </c>
       <c r="G25" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -13891,7 +14585,7 @@
         <v>150</v>
       </c>
       <c r="G26" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -13912,7 +14606,7 @@
         <v>150</v>
       </c>
       <c r="G27" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -13933,7 +14627,7 @@
         <v>150</v>
       </c>
       <c r="G28" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -13954,7 +14648,7 @@
         <v>150</v>
       </c>
       <c r="G29" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -13975,7 +14669,7 @@
         <v>150</v>
       </c>
       <c r="G30" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -13996,7 +14690,7 @@
         <v>167</v>
       </c>
       <c r="G31" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -14017,7 +14711,7 @@
         <v>150</v>
       </c>
       <c r="G32" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -14038,7 +14732,7 @@
         <v>150</v>
       </c>
       <c r="G33" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -14059,7 +14753,7 @@
         <v>150</v>
       </c>
       <c r="G34" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -14080,7 +14774,7 @@
         <v>150</v>
       </c>
       <c r="G35" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -14101,7 +14795,7 @@
         <v>150</v>
       </c>
       <c r="G36" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -14122,7 +14816,7 @@
         <v>150</v>
       </c>
       <c r="G37" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -14143,7 +14837,7 @@
         <v>150</v>
       </c>
       <c r="G38" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -14164,7 +14858,7 @@
         <v>150</v>
       </c>
       <c r="G39" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -14185,7 +14879,7 @@
         <v>150</v>
       </c>
       <c r="G40" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -14206,7 +14900,7 @@
         <v>167</v>
       </c>
       <c r="G41" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -14227,7 +14921,7 @@
         <v>223</v>
       </c>
       <c r="G42" s="11">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
datatool latest changes and import files
</commit_message>
<xml_diff>
--- a/files/DxH_ConfigImport_Veniano_HA.xlsx
+++ b/files/DxH_ConfigImport_Veniano_HA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rf128sp\ADV-DXH\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6591B280-5EA1-4655-A697-CC05FF6B40B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BD43A7-6112-4979-80C4-96099BBB0194}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dtreason" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="245">
   <si>
     <t>asset_code</t>
   </si>
@@ -764,6 +764,9 @@
   </si>
   <si>
     <t>168H-0003.Cutter.Count</t>
+  </si>
+  <si>
+    <t>decimals</t>
   </si>
 </sst>
 </file>
@@ -10959,10 +10962,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10977,7 +10980,7 @@
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
@@ -11008,8 +11011,11 @@
       <c r="J1" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -11039,6 +11045,9 @@
       </c>
       <c r="J2">
         <v>119</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -14027,7 +14036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868E2915-FB4F-49BC-B896-6E22979130DF}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>

</xml_diff>